<commit_message>
Last minute cancellation - updated registration list
</commit_message>
<xml_diff>
--- a/assets/files/all-registered-final.xlsx
+++ b/assets/files/all-registered-final.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="620" windowWidth="25360" windowHeight="15380"/>
+    <workbookView xWindow="7440" yWindow="2020" windowWidth="25360" windowHeight="15380"/>
   </bookViews>
   <sheets>
     <sheet name="Registration NeIC AllHandsMeeti" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="271">
   <si>
     <t>First name</t>
   </si>
@@ -588,15 +588,6 @@
   </si>
   <si>
     <t>CSC - IT Center for Science Ltd.</t>
-  </si>
-  <si>
-    <t>minna.ahokas@csc.fi</t>
-  </si>
-  <si>
-    <t>Minna</t>
-  </si>
-  <si>
-    <t>Ahokas</t>
   </si>
   <si>
     <t>tommi.jalkanen@csc.fi</t>
@@ -1272,10 +1263,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="E77" sqref="E77"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1291,22 +1282,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1323,10 +1314,10 @@
         <v>2</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1346,7 +1337,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.2">
@@ -1363,7 +1354,7 @@
         <v>13</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>6</v>
@@ -1466,7 +1457,7 @@
         <v>5</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1526,7 +1517,7 @@
         <v>5</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1586,7 +1577,7 @@
         <v>52</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1703,10 +1694,10 @@
         <v>82</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -1723,10 +1714,10 @@
         <v>85</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -1823,10 +1814,10 @@
         <v>103</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -2263,7 +2254,7 @@
         <v>178</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>67</v>
@@ -2329,7 +2320,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -2343,13 +2334,13 @@
         <v>190</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>52</v>
+        <v>186</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -2363,13 +2354,13 @@
         <v>193</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>186</v>
+        <v>52</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -2383,30 +2374,30 @@
         <v>196</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>52</v>
+        <v>199</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D56" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>199</v>
-      </c>
       <c r="E56" s="4" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -2414,39 +2405,39 @@
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D57" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>203</v>
-      </c>
       <c r="E57" s="4" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D58" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="C58" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>207</v>
-      </c>
       <c r="E58" s="4" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>256</v>
+        <v>67</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -2454,13 +2445,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>212</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>211</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>214</v>
@@ -2477,16 +2468,16 @@
         <v>216</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>115</v>
+        <v>217</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>215</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>67</v>
+        <v>254</v>
       </c>
     </row>
     <row r="61" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -2494,19 +2485,19 @@
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D61" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="C61" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>218</v>
-      </c>
       <c r="E61" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>257</v>
+        <v>12</v>
       </c>
     </row>
     <row r="62" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -2514,22 +2505,22 @@
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="D62" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="C62" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>222</v>
-      </c>
       <c r="E62" s="4" t="s">
-        <v>225</v>
+        <v>154</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -2543,7 +2534,7 @@
         <v>226</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>154</v>
+        <v>52</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>67</v>
@@ -2569,7 +2560,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="65" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -2583,13 +2574,13 @@
         <v>232</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -2603,10 +2594,10 @@
         <v>235</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>33</v>
+        <v>238</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>272</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -2614,22 +2605,22 @@
         <v>66</v>
       </c>
       <c r="B67" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D67" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="C67" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>238</v>
-      </c>
       <c r="E67" s="4" t="s">
-        <v>241</v>
+        <v>146</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -2643,10 +2634,10 @@
         <v>242</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>146</v>
+        <v>245</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
     </row>
     <row r="69" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -2654,38 +2645,18 @@
         <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="D69" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="C69" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>245</v>
-      </c>
       <c r="E69" s="4" t="s">
-        <v>248</v>
+        <v>270</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="2">
-        <v>69</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="F70" s="5" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>